<commit_message>
Ordering content of folders, added comments to schedule documentation
</commit_message>
<xml_diff>
--- a/doc/start-14-pl-06/start-14-pl-06.xlsx
+++ b/doc/start-14-pl-06/start-14-pl-06.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Tydzień</t>
   </si>
@@ -164,6 +164,24 @@
   </si>
   <si>
     <t>Metodologia: Unified Process</t>
+  </si>
+  <si>
+    <t>Po zapoznaniu się z dokumentacją, konieczne było wyjaśnienie paru niejasności z prowadzącymi przedmiot (1h). Przedyskutowanie problemu z grupą (2h).</t>
+  </si>
+  <si>
+    <t>Założenie repozytorium zgodnie z zaleceniami (2h). Stworzenie szkieletu klienta (1h).</t>
+  </si>
+  <si>
+    <t>Stworzenie całego klienta (wersja niedziałająca). Ponadto opracowanie części projektu Common wspólnego dla wielu komponentów (całość 3h).</t>
+  </si>
+  <si>
+    <t>Dopracowanie clienta - wersja poprawnie nawiązująca połączenie i wysyłająca cokolwiek (3h). Nadprogramowe (2h) na poprawki związane ze zmianą sposobu komunikacji.</t>
+  </si>
+  <si>
+    <t>Dopracowanie clienta - wersja działająca także z serwerami innych zespołów (3h). Nadprogramowe (6h) związane z ponowną zmianą sposobu komunikacji. Kolejne (4h) więcej na stworzenie dokumentacji oraz UnitTestów.</t>
+  </si>
+  <si>
+    <t>Ostatnie poprawki, zwłaszcza w wyglądzie kodu. Poprawienie drobnych błędów. (Całość 3h)</t>
   </si>
 </sst>
 </file>
@@ -912,8 +930,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1015,9 +1033,11 @@
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1036,9 +1056,11 @@
       <c r="H6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1057,9 +1079,11 @@
       <c r="H7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1078,9 +1102,11 @@
       <c r="H8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1099,9 +1125,11 @@
       <c r="H9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1120,9 +1148,11 @@
       <c r="H10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -1143,7 +1173,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -1164,7 +1194,7 @@
       </c>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1185,7 +1215,7 @@
       </c>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -1206,7 +1236,7 @@
       </c>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -1227,7 +1257,7 @@
       </c>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -1248,7 +1278,7 @@
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -1269,7 +1299,7 @@
       </c>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -1302,6 +1332,6 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="4" scale="91" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="4" scale="57" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filled time tracking excel file
</commit_message>
<xml_diff>
--- a/doc/start-14-pl-06/start-14-pl-06.xlsx
+++ b/doc/start-14-pl-06/start-14-pl-06.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="63">
   <si>
     <t>Tydzień</t>
   </si>
@@ -82,12 +82,6 @@
     <t>Championship (3h)</t>
   </si>
   <si>
-    <t>Wstępna implementacja i projektowanie komunikacji - Task Solver (3h)</t>
-  </si>
-  <si>
-    <t>Testowanie komunikacji - Task Solver (3h)</t>
-  </si>
-  <si>
     <t>Działająca komunikacja pomiędzy innymi komponentami aplikacji</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>Działający algorytm</t>
   </si>
   <si>
-    <t>Testowanie i implementacja  pozostałych funkcjonalności - Task Solver (3h)</t>
-  </si>
-  <si>
     <t>Testowanie - Task Solver (3h)</t>
   </si>
   <si>
@@ -182,6 +173,39 @@
   </si>
   <si>
     <t>Ostatnie poprawki, zwłaszcza w wyglądzie kodu. Poprawienie drobnych błędów. (Całość 3h)</t>
+  </si>
+  <si>
+    <t>Projektowanie architektury wspólnej komunikacji (Network Adapter używany w komponentach poza serwerem)</t>
+  </si>
+  <si>
+    <t>Stworzenie szkieletu Task Managera.</t>
+  </si>
+  <si>
+    <t>Wstępna implementacja i projektowanie komunikacji - Task Manager (3h)</t>
+  </si>
+  <si>
+    <t>Dopracowywanie komunikacji - Task manger (3h)</t>
+  </si>
+  <si>
+    <t>Testowanie komunikacji - Task Manager (3h)</t>
+  </si>
+  <si>
+    <t>Testowanie i implementacja  pozostałych funkcjonalności - Task Manager (3h)</t>
+  </si>
+  <si>
+    <t>Testowanie - Task manger (3h)</t>
+  </si>
+  <si>
+    <t>Projektowanie i impementacja Task Managera, Netrok Adaptera.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eksport kodu do nowego repozytorium svn. Projektowanie i impementacja Task Managera, Netrok Adaptera. </t>
+  </si>
+  <si>
+    <t>Zmiana w sposobie komunikacji w serwerze, spowodowana ustaleniami z innymi grupami. Unit testy.</t>
+  </si>
+  <si>
+    <t>Refaktoryzacja kodu.</t>
   </si>
 </sst>
 </file>
@@ -623,7 +647,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -639,9 +663,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -679,7 +703,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -751,7 +775,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -930,8 +954,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +979,7 @@
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -1021,7 +1045,9 @@
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1034,7 +1060,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1042,11 +1068,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="15"/>
+        <v>54</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="D6" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="11" t="s">
@@ -1054,10 +1082,10 @@
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1065,11 +1093,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="D7" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="11" t="s">
@@ -1077,10 +1107,10 @@
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1088,11 +1118,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="D8" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="11" t="s">
@@ -1100,10 +1132,10 @@
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1111,11 +1143,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="D9" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="11" t="s">
@@ -1123,10 +1157,10 @@
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1134,22 +1168,24 @@
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="15"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="D10" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1157,11 +1193,11 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="11" t="s">
@@ -1169,7 +1205,7 @@
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I11" s="10"/>
     </row>
@@ -1178,11 +1214,11 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="11" t="s">
@@ -1190,7 +1226,7 @@
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I12" s="10"/>
     </row>
@@ -1199,11 +1235,11 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="11" t="s">
@@ -1211,7 +1247,7 @@
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I13" s="10"/>
     </row>
@@ -1220,11 +1256,11 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="11" t="s">
@@ -1232,7 +1268,7 @@
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I14" s="10"/>
     </row>
@@ -1241,11 +1277,11 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="11" t="s">
@@ -1253,7 +1289,7 @@
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I15" s="10"/>
     </row>
@@ -1262,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="9" t="s">

</xml_diff>

<commit_message>
Added commemts to work plan in doc
</commit_message>
<xml_diff>
--- a/doc/start-14-pl-06/start-14-pl-06.xlsx
+++ b/doc/start-14-pl-06/start-14-pl-06.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>Tydzień</t>
   </si>
@@ -206,6 +206,21 @@
   </si>
   <si>
     <t>Refaktoryzacja kodu.</t>
+  </si>
+  <si>
+    <t>Pytania odnośnie dokumentacji i podział prac w grupie. Projektowanie biblioteki dla całego zespołu (3h)</t>
+  </si>
+  <si>
+    <t>Stworzenie szkieletu serwera i dokończenie biblioteki (3h)</t>
+  </si>
+  <si>
+    <t>Implementacja odbierania i wysyłania wiadomości (3h)</t>
+  </si>
+  <si>
+    <t>Implementacja prostego algorytmu rozdzielającego zadania pomiędzy komponenty (3h)</t>
+  </si>
+  <si>
+    <t>Wprowadzanie poprawek zauważonych podczas testów (3h)</t>
   </si>
 </sst>
 </file>
@@ -647,7 +662,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -663,9 +678,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -703,7 +718,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -775,7 +790,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -955,7 +970,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1066,9 @@
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="F5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1093,9 @@
       <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="F6" s="11" t="s">
         <v>9</v>
       </c>
@@ -1101,7 +1120,9 @@
       <c r="D7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1147,9 @@
       <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1174,9 @@
       <c r="D9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="F9" s="11" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added comments to work plan
</commit_message>
<xml_diff>
--- a/doc/start-14-pl-06/start-14-pl-06.xlsx
+++ b/doc/start-14-pl-06/start-14-pl-06.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Arkusz1!$A$1:$I$18</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>Tydzień</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t>Wprowadzanie poprawek zauważonych podczas testów (3h)</t>
+  </si>
+  <si>
+    <t>Stworzenie szkieletu Computational Noda(3h).</t>
+  </si>
+  <si>
+    <t>Zapoznanie się z dokumentacją, wyjaśnienie niejasność. Podział prac w grupie(3h).</t>
+  </si>
+  <si>
+    <t>Projektowanie i implementacja Computational Noda(3h).</t>
+  </si>
+  <si>
+    <t>Wprowadzenie poprawek zwiazanych ze zmianą sposobu komunikacji(dodatkowe 4h).</t>
   </si>
 </sst>
 </file>
@@ -720,7 +732,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,7 +767,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -969,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1084,9 @@
       <c r="F5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1099,7 +1113,9 @@
       <c r="F6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="H6" s="9" t="s">
         <v>25</v>
       </c>
@@ -1126,7 +1142,9 @@
       <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="H7" s="11" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1171,9 @@
       <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="H8" s="11" t="s">
         <v>26</v>
       </c>
@@ -1180,7 +1200,9 @@
       <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="H9" s="11" t="s">
         <v>30</v>
       </c>
@@ -1205,7 +1227,9 @@
       <c r="F10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Update project status file
</commit_message>
<xml_diff>
--- a/doc/start-14-pl-06/start-14-pl-06.xlsx
+++ b/doc/start-14-pl-06/start-14-pl-06.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>Tydzień</t>
   </si>
@@ -233,6 +233,18 @@
   </si>
   <si>
     <t>Wprowadzenie poprawek zwiazanych ze zmianą sposobu komunikacji(dodatkowe 4h).</t>
+  </si>
+  <si>
+    <t>Refaktoryzacja kodu</t>
+  </si>
+  <si>
+    <t>Implementacja metod Merge i Divide. Integracja z komponentami</t>
+  </si>
+  <si>
+    <t>Popawki wydajnościowe w komunikacji oraz w metodach wtyczki</t>
+  </si>
+  <si>
+    <t>Implementacja metod Merge i Divide. Integracja z komponentami innych grup</t>
   </si>
 </sst>
 </file>
@@ -674,7 +686,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -690,9 +702,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -730,9 +742,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -767,7 +779,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -802,7 +814,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -981,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1235,9 @@
       <c r="D10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1244,11 +1258,15 @@
       <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="D11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1265,11 +1283,15 @@
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="D12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F12" s="11" t="s">
         <v>14</v>
       </c>
@@ -1286,11 +1308,15 @@
       <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="D13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1307,11 +1333,15 @@
       <c r="B14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="D14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F14" s="11" t="s">
         <v>16</v>
       </c>
@@ -1328,11 +1358,15 @@
       <c r="B15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="D15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F15" s="11" t="s">
         <v>17</v>
       </c>
@@ -1349,11 +1383,15 @@
       <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="D16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F16" s="11" t="s">
         <v>18</v>
       </c>
@@ -1370,11 +1408,15 @@
       <c r="B17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="D17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="F17" s="11" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Fixed probelm with excel file
</commit_message>
<xml_diff>
--- a/doc/start-14-pl-06/start-14-pl-06.xlsx
+++ b/doc/start-14-pl-06/start-14-pl-06.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>Tydzień</t>
   </si>
@@ -254,6 +254,33 @@
   </si>
   <si>
     <t>Testowanie działania algorytmu wraz z komponentami w zakresie grupy oraz naniesienie odpowiednich poprawek (3h).</t>
+  </si>
+  <si>
+    <t>Implementacja metod Merge i Divide. Integracja z komponentami</t>
+  </si>
+  <si>
+    <t>Popawki wydajnościowe w komunikacji oraz w metodach wtyczki</t>
+  </si>
+  <si>
+    <t>Implementacja metod Merge i Divide. Integracja z komponentami innych grup</t>
+  </si>
+  <si>
+    <t>Praca nad szablonem algorytmu.</t>
+  </si>
+  <si>
+    <t>Praca nad algorytmem.</t>
+  </si>
+  <si>
+    <t>Testowanie algorytmu.</t>
+  </si>
+  <si>
+    <t>Dodanie brakujacych funkcjonalności.</t>
+  </si>
+  <si>
+    <t>Testowanie połączenia z innymi grupami.</t>
+  </si>
+  <si>
+    <t>Refaktoryzacja kodu</t>
   </si>
 </sst>
 </file>
@@ -617,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -663,6 +690,15 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,7 +731,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -711,9 +747,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -751,7 +787,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -823,7 +859,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1002,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E18" sqref="E5:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,54 +1049,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1099,13 +1135,13 @@
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="17" t="s">
         <v>63</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="17" t="s">
         <v>69</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -1128,13 +1164,13 @@
       <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="18" t="s">
         <v>64</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="18" t="s">
         <v>68</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -1157,13 +1193,13 @@
       <c r="D7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="18" t="s">
         <v>70</v>
       </c>
       <c r="H7" s="11" t="s">
@@ -1186,13 +1222,13 @@
       <c r="D8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="18" t="s">
         <v>66</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="18" t="s">
         <v>70</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -1215,13 +1251,13 @@
       <c r="D9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="18" t="s">
         <v>67</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="18" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -1244,11 +1280,13 @@
       <c r="D10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="18" t="s">
         <v>62</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1265,15 +1303,21 @@
       <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="D11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="H11" s="11" t="s">
         <v>36</v>
       </c>
@@ -1288,15 +1332,21 @@
       <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="D12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="H12" s="9" t="s">
         <v>37</v>
       </c>
@@ -1311,15 +1361,21 @@
       <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="D13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="H13" s="9" t="s">
         <v>40</v>
       </c>
@@ -1334,15 +1390,21 @@
       <c r="B14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>80</v>
+      </c>
       <c r="D14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="H14" s="11" t="s">
         <v>41</v>
       </c>
@@ -1357,15 +1419,21 @@
       <c r="B15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="H15" s="9" t="s">
         <v>43</v>
       </c>
@@ -1380,15 +1448,21 @@
       <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="H16" s="11" t="s">
         <v>18</v>
       </c>
@@ -1403,15 +1477,21 @@
       <c r="B17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="F17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="H17" s="11" t="s">
         <v>19</v>
       </c>
@@ -1430,11 +1510,11 @@
       <c r="D18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="16"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="12" t="s">
         <v>20</v>
       </c>

</xml_diff>